<commit_message>
BPA cohort 3 update
</commit_message>
<xml_diff>
--- a/data/echoMRI/Kotz01212026.xlsx
+++ b/data/echoMRI/Kotz01212026.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
   <workbookPr backupFile="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcab/Documents/GitHub/data/data/echoMRI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4B5DE9A-EB57-8146-8328-057150D44FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE760F61-A85F-2C4D-8741-961CB927B896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="44800" windowHeight="25200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,73 +124,73 @@
     <t>9453</t>
   </si>
   <si>
-    <t>13:17:48 Jan 21, 2026; 31; ems</t>
-  </si>
-  <si>
-    <t>13:19:38 Jan 21, 2026; 31; ems</t>
-  </si>
-  <si>
-    <t>13:21:18 Jan 21, 2026; 27; ems</t>
-  </si>
-  <si>
-    <t>13:22:52 Jan 21, 2026; 36; ems</t>
-  </si>
-  <si>
-    <t>13:24:54 Jan 21, 2026; 27; ems</t>
-  </si>
-  <si>
-    <t>13:26:34 Jan 21, 2026; 31; ems</t>
-  </si>
-  <si>
-    <t>13:27:59 Jan 21, 2026; 27; ems</t>
-  </si>
-  <si>
-    <t>13:29:24 Jan 21, 2026; 27; ems</t>
-  </si>
-  <si>
-    <t>13:30:34 Jan 21, 2026; 31; ems</t>
-  </si>
-  <si>
-    <t>13:31:48 Jan 21, 2026; 31; ems</t>
-  </si>
-  <si>
-    <t>13:33:14 Jan 21, 2026; 36; ems</t>
-  </si>
-  <si>
-    <t>13:35:23 Jan 21, 2026; 31; ems</t>
-  </si>
-  <si>
-    <t>13:36:35 Jan 21, 2026; 36; ems</t>
-  </si>
-  <si>
-    <t>13:39:04 Jan 21, 2026; 36; ems</t>
-  </si>
-  <si>
-    <t>13:40:36 Jan 21, 2026; 31; ems</t>
-  </si>
-  <si>
-    <t>13:42:07 Jan 21, 2026; 31; ems</t>
-  </si>
-  <si>
-    <t>13:43:31 Jan 21, 2026; 27; ems</t>
-  </si>
-  <si>
-    <t>13:45:08 Jan 21, 2026; 31; ems</t>
-  </si>
-  <si>
-    <t>13:46:48 Jan 21, 2026; 31; ems</t>
-  </si>
-  <si>
-    <t>13:48:18 Jan 21, 2026; 31; ems</t>
-  </si>
-  <si>
-    <t>13:49:35 Jan 21, 2026; 32; ems</t>
-  </si>
-  <si>
-    <t>13:51:12 Jan 21, 2026; 32; ems</t>
-  </si>
-  <si>
-    <t>13:52:25 Jan 21, 2026; 31; ems</t>
+    <t>13:17:48 21 Jan, 2026; 31; ems</t>
+  </si>
+  <si>
+    <t>13:19:38 21 Jan, 2026; 31; ems</t>
+  </si>
+  <si>
+    <t>13:21:18 21 Jan, 2026; 27; ems</t>
+  </si>
+  <si>
+    <t>13:22:52 21 Jan, 2026; 36; ems</t>
+  </si>
+  <si>
+    <t>13:24:54 21 Jan, 2026; 27; ems</t>
+  </si>
+  <si>
+    <t>13:26:34 21 Jan, 2026; 31; ems</t>
+  </si>
+  <si>
+    <t>13:27:59 21 Jan, 2026; 27; ems</t>
+  </si>
+  <si>
+    <t>13:29:24 21 Jan, 2026; 27; ems</t>
+  </si>
+  <si>
+    <t>13:30:34 21 Jan, 2026; 31; ems</t>
+  </si>
+  <si>
+    <t>13:31:48 21 Jan, 2026; 31; ems</t>
+  </si>
+  <si>
+    <t>13:33:14 21 Jan, 2026; 36; ems</t>
+  </si>
+  <si>
+    <t>13:35:23 21 Jan, 2026; 31; ems</t>
+  </si>
+  <si>
+    <t>13:36:35 21 Jan, 2026; 36; ems</t>
+  </si>
+  <si>
+    <t>13:39:04 21 Jan, 2026; 36; ems</t>
+  </si>
+  <si>
+    <t>13:40:36 21 Jan, 2026; 31; ems</t>
+  </si>
+  <si>
+    <t>13:42:07 21 Jan, 2026; 31; ems</t>
+  </si>
+  <si>
+    <t>13:43:31 21 Jan, 2026; 27; ems</t>
+  </si>
+  <si>
+    <t>13:45:08 21 Jan, 2026; 31; ems</t>
+  </si>
+  <si>
+    <t>13:46:48 21 Jan, 2026; 31; ems</t>
+  </si>
+  <si>
+    <t>13:48:18 21 Jan, 2026; 31; ems</t>
+  </si>
+  <si>
+    <t>13:49:35 21 Jan, 2026; 32; ems</t>
+  </si>
+  <si>
+    <t>13:51:12 21 Jan, 2026; 32; ems</t>
+  </si>
+  <si>
+    <t>13:52:25 21 Jan, 2026; 31; ems</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="7" max="7" width="25.19921875" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">

</xml_diff>